<commit_message>
Agregue para editar articulos
</commit_message>
<xml_diff>
--- a/lista.xlsx
+++ b/lista.xlsx
@@ -1,28 +1,51 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26707"/>
   <workbookPr/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2EF76966-51EB-4318-843B-C72F0FF1E5B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Hoja 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>id</t>
   </si>
   <si>
-    <t>Alimento</t>
-  </si>
-  <si>
-    <t>Tipo</t>
-  </si>
-  <si>
-    <t>Precio</t>
+    <t>alimento</t>
+  </si>
+  <si>
+    <t>tipo</t>
+  </si>
+  <si>
+    <t>precio</t>
+  </si>
+  <si>
+    <t>peso</t>
+  </si>
+  <si>
+    <t>stock</t>
   </si>
   <si>
     <t>Nutribon</t>
@@ -43,16 +66,24 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -62,36 +93,44 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -281,20 +320,25 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -307,50 +351,77 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D2" s="1">
-        <v>2000.0</v>
+        <v>2700</v>
+      </c>
+      <c r="E2">
+        <v>8</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D3" s="1">
-        <v>10000.0</v>
+        <v>9000</v>
+      </c>
+      <c r="E3">
+        <v>21</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1">
-        <v>2000.0</v>
-      </c>
+        <v>8900</v>
+      </c>
+      <c r="E4">
+        <v>15</v>
+      </c>
+      <c r="F4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" customHeight="1">
+      <c r="J11" s="2"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
agregue la posibilidad de eliminar ventas y corregi unas cositas
</commit_message>
<xml_diff>
--- a/lista.xlsx
+++ b/lista.xlsx
@@ -397,187 +397,257 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
+        <v>id</v>
+      </c>
+      <c r="B1" t="str">
         <v>name</v>
-      </c>
-      <c r="B1" t="str">
-        <v>tipo</v>
       </c>
       <c r="C1" t="str">
         <v>peso</v>
       </c>
       <c r="D1" t="str">
+        <v>tipo</v>
+      </c>
+      <c r="E1" t="str">
         <v>price</v>
       </c>
-      <c r="E1" t="str">
+      <c r="F1" t="str">
+        <v>precioSuelto</v>
+      </c>
+      <c r="G1" t="str">
         <v>stock</v>
       </c>
-      <c r="F1" t="str">
+      <c r="H1" t="str">
         <v>fechaActualizacion</v>
       </c>
-      <c r="G1" t="str">
-        <v>id</v>
-      </c>
-      <c r="H1" t="str">
+      <c r="I1" t="str">
         <v>tipoEdad</v>
       </c>
-      <c r="I1" t="str">
+      <c r="J1" t="str">
         <v>tipoMordida</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="str">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="str">
         <v>DOGUI</v>
       </c>
-      <c r="B2" t="str">
+      <c r="C2">
+        <v>23</v>
+      </c>
+      <c r="D2" t="str">
         <v>PERRO</v>
       </c>
-      <c r="C2" t="str">
+      <c r="E2">
         <v>23</v>
       </c>
-      <c r="D2" t="str">
+      <c r="F2">
+        <v>20</v>
+      </c>
+      <c r="G2">
         <v>23</v>
       </c>
-      <c r="E2" t="str">
-        <v>23</v>
-      </c>
-      <c r="F2" t="str">
-        <v>2023-09-07</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
+      <c r="H2" t="str">
+        <v>2023-09-08</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="str">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
         <v>NUTRIBON</v>
-      </c>
-      <c r="B3" t="str">
-        <v>PERRO</v>
       </c>
       <c r="C3" t="str">
         <v>20</v>
       </c>
       <c r="D3" t="str">
-        <v>31</v>
+        <v>PERRO</v>
       </c>
       <c r="E3" t="str">
         <v>31</v>
       </c>
-      <c r="F3" t="str">
+      <c r="G3" t="str">
+        <v>31</v>
+      </c>
+      <c r="H3" t="str">
         <v>2023-09-07</v>
       </c>
-      <c r="G3">
-        <v>2</v>
-      </c>
     </row>
     <row r="4">
-      <c r="A4" t="str">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="str">
         <v>A</v>
       </c>
-      <c r="B4" t="str">
+      <c r="C4" t="str">
+        <v>123</v>
+      </c>
+      <c r="D4" t="str">
         <v>PERRO</v>
       </c>
-      <c r="C4" t="str">
-        <v>123</v>
-      </c>
-      <c r="D4" t="str">
-        <v>123</v>
-      </c>
       <c r="E4" t="str">
         <v>123</v>
       </c>
-      <c r="F4" t="str">
+      <c r="G4" t="str">
+        <v>123</v>
+      </c>
+      <c r="H4" t="str">
         <v>2023-09-07</v>
       </c>
-      <c r="G4">
-        <v>3</v>
-      </c>
     </row>
     <row r="5">
-      <c r="A5" t="str">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="str">
         <v>B</v>
       </c>
-      <c r="B5" t="str">
+      <c r="C5" t="str">
+        <v>123</v>
+      </c>
+      <c r="D5" t="str">
         <v>PERRO</v>
       </c>
-      <c r="C5" t="str">
-        <v>123</v>
-      </c>
-      <c r="D5" t="str">
-        <v>123</v>
-      </c>
       <c r="E5" t="str">
         <v>123</v>
       </c>
-      <c r="F5" t="str">
+      <c r="G5" t="str">
+        <v>123</v>
+      </c>
+      <c r="H5" t="str">
         <v>2023-09-07</v>
       </c>
-      <c r="G5">
-        <v>4</v>
-      </c>
     </row>
     <row r="6">
-      <c r="A6" t="str">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="str">
         <v>NUTRIBON</v>
-      </c>
-      <c r="B6" t="str">
-        <v>GATO</v>
       </c>
       <c r="C6" t="str">
         <v>8</v>
       </c>
       <c r="D6" t="str">
+        <v>GATO</v>
+      </c>
+      <c r="E6" t="str">
         <v>10000</v>
       </c>
-      <c r="E6" t="str">
+      <c r="G6" t="str">
         <v>1</v>
       </c>
-      <c r="F6" t="str">
+      <c r="H6" t="str">
         <v>2023-09-07</v>
       </c>
-      <c r="G6">
-        <v>5</v>
-      </c>
     </row>
     <row r="7">
-      <c r="A7" t="str">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="str">
         <v>NUTRIBON</v>
-      </c>
-      <c r="B7" t="str">
-        <v>PERRO</v>
       </c>
       <c r="C7" t="str">
         <v>12</v>
       </c>
       <c r="D7" t="str">
+        <v>PERRO</v>
+      </c>
+      <c r="E7" t="str">
         <v>123123</v>
       </c>
-      <c r="E7" t="str">
+      <c r="G7" t="str">
         <v>22</v>
       </c>
-      <c r="F7" t="str">
+      <c r="H7" t="str">
         <v>2023-09-07</v>
       </c>
-      <c r="G7">
-        <v>6</v>
-      </c>
-      <c r="H7" t="str">
+      <c r="I7" t="str">
         <v>ADULTO</v>
       </c>
-      <c r="I7" t="str">
+      <c r="J7" t="str">
         <v>GRANDE</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="str">
+        <v>JUAN</v>
+      </c>
+      <c r="C8" t="str">
+        <v>2</v>
+      </c>
+      <c r="D8" t="str">
+        <v>PERRO</v>
+      </c>
+      <c r="E8" t="str">
+        <v>1777</v>
+      </c>
+      <c r="F8" t="str">
+        <v>23</v>
+      </c>
+      <c r="G8" t="str">
+        <v>1</v>
+      </c>
+      <c r="H8" t="str">
+        <v>2023-09-08</v>
+      </c>
+      <c r="I8" t="str">
+        <v>CACHORRO</v>
+      </c>
+      <c r="J8" t="str">
+        <v>GRANDE</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="str">
+        <v>ASD</v>
+      </c>
+      <c r="C9" t="str">
+        <v>10</v>
+      </c>
+      <c r="D9" t="str">
+        <v>PERRO</v>
+      </c>
+      <c r="E9" t="str">
+        <v>123</v>
+      </c>
+      <c r="F9" t="str">
+        <v>123</v>
+      </c>
+      <c r="G9" t="str">
+        <v>123</v>
+      </c>
+      <c r="H9" t="str">
+        <v>2023-09-08</v>
+      </c>
+      <c r="I9" t="str">
+        <v>-</v>
+      </c>
+      <c r="J9" t="str">
+        <v>-</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:J9"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
arranque a armar caja mensual
</commit_message>
<xml_diff>
--- a/lista.xlsx
+++ b/lista.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -677,9 +677,49 @@
         <v>GRANDE</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="H11" t="str">
+        <v>2023-09-11</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="H12" t="str">
+        <v>2023-09-11</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="H13" t="str">
+        <v>2023-09-11</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="H14" t="str">
+        <v>2023-09-11</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="H15" t="str">
+        <v>2023-09-11</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:J10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:J15"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Corregi error actualizar articulo
</commit_message>
<xml_diff>
--- a/lista.xlsx
+++ b/lista.xlsx
@@ -559,20 +559,23 @@
       <c r="B7" t="str">
         <v>NUTRIBON</v>
       </c>
-      <c r="C7" t="str">
+      <c r="C7">
         <v>12</v>
       </c>
       <c r="D7" t="str">
         <v>PERRO</v>
       </c>
-      <c r="E7" t="str">
+      <c r="E7">
         <v>123123</v>
       </c>
-      <c r="G7" t="str">
-        <v>22</v>
+      <c r="F7">
+        <v>20</v>
+      </c>
+      <c r="G7">
+        <v>999</v>
       </c>
       <c r="H7" t="str">
-        <v>2023-09-07</v>
+        <v>2023-10-03</v>
       </c>
       <c r="I7" t="str">
         <v>ADULTO</v>

</xml_diff>